<commit_message>
updated template API logic add
</commit_message>
<xml_diff>
--- a/data/config_data.xlsx
+++ b/data/config_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesys1_onmicrosoft_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC423B5-7B7E-40C5-9BB2-B063E8D71967}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC2B8BC-B58B-4331-98AD-FBD21C6E1CE6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,34 +444,34 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case Report Excel and API DB connection add
</commit_message>
<xml_diff>
--- a/data/config_data.xlsx
+++ b/data/config_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesys1_onmicrosoft_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC2B8BC-B58B-4331-98AD-FBD21C6E1CE6}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD8D9A67-B1B5-4810-96CB-A2DF2124D4D7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>ppapplicationurl</t>
+  </si>
+  <si>
+    <t>PP_2_6_3_B2_P2</t>
+  </si>
+  <si>
+    <t>Playwright_test_set</t>
+  </si>
+  <si>
+    <t>feature_name</t>
+  </si>
+  <si>
+    <t>build_version</t>
   </si>
 </sst>
 </file>
@@ -398,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +486,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Developed Test Cases - Learning & Development
</commit_message>
<xml_diff>
--- a/data/config_data.xlsx
+++ b/data/config_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesys1_onmicrosoft_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiac\OneDrive - Walker Digital Table Systems\PlayWright_Project\PlayWright_POC\PlayWright_POC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC423B5-7B7E-40C5-9BB2-B063E8D71967}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0344B3-5FBC-4760-8369-0CAAE5B26236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,16 +401,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -418,7 +418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -426,7 +426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -434,7 +434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -450,7 +450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
remove argument in the updated system tab
</commit_message>
<xml_diff>
--- a/data/config_data.xlsx
+++ b/data/config_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesystems-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWright_POC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EF8A02C-5C24-45AC-8ED4-EA099FC7AB60}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{839A5068-DD51-4FBB-A02D-FF2E3A777393}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>browser</t>
   </si>
   <si>
-    <t>edge</t>
-  </si>
-  <si>
     <t>env</t>
   </si>
   <si>
@@ -69,22 +66,26 @@
     <t>ppapplicationurl</t>
   </si>
   <si>
-    <t>Playwright_test_set</t>
-  </si>
-  <si>
     <t>feature_name</t>
   </si>
   <si>
     <t>build_version</t>
   </si>
   <si>
-    <t>aut02</t>
-  </si>
-  <si>
-    <t>PP_2_6_4_B1</t>
-  </si>
-  <si>
-    <t>172.41.46.26</t>
+    <t>172.41.46.23</t>
+  </si>
+  <si>
+    <t>cs01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PP_2_6_3_B2_P2</t>
+  </si>
+  <si>
+    <t>Playwright_POC</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -413,7 +414,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +436,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,15 +444,15 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,10 +473,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,18 +489,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>